<commit_message>
Adding final clean data and updating references to data in JS
</commit_message>
<xml_diff>
--- a/data/International_Population_By_Country.xlsx
+++ b/data/International_Population_By_Country.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gisselle.frias/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gisselle.frias/Sites/sotu-carbon/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8140008_{55D26B81-FBC5-9541-AF0E-7E229BDFD74B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{359049CC-A732-384C-A396-9F6C0BF813B0}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3620" yWindow="-21080" windowWidth="28780" windowHeight="17840" activeTab="3"/>
+    <workbookView xWindow="7360" yWindow="-19740" windowWidth="28780" windowHeight="17840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="International_Population_By_Cou" sheetId="1" r:id="rId1"/>
     <sheet name="International_Population_By (2)" sheetId="2" r:id="rId2"/>
     <sheet name="Transposed" sheetId="3" r:id="rId3"/>
-    <sheet name="Transposed x 1000 + IEA report" sheetId="4" r:id="rId4"/>
+    <sheet name="Transposed x 1000 + IEA country" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
@@ -757,7 +757,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1620,11 +1620,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O235"/>
   <sheetViews>
-    <sheetView topLeftCell="A185" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="A196" sqref="A196:XFD196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11738,7 +11738,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M229"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -21142,7 +21142,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:HU13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -30119,11 +30119,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:EM13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="DV1" workbookViewId="0">
-      <selection activeCell="V1" sqref="V1:V1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="19" x14ac:dyDescent="0.25"/>

</xml_diff>